<commit_message>
Minor updates and clear all cells
</commit_message>
<xml_diff>
--- a/notebooks/data/excel/triangle_data.xlsx
+++ b/notebooks/data/excel/triangle_data.xlsx
@@ -18,11 +18,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
     <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
     <numFmt numFmtId="166" formatCode="yyyy-mm-dd"/>
-    <numFmt numFmtId="167" formatCode="YYYY-MM-DD"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -68,7 +67,7 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -460,22 +459,22 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>line_of_busines</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>reinsurance_basis</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>risk_basis</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
           <t>loss_definition</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>line_of_busines</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>risk_basis</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>reinsurance_basis</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
@@ -503,12 +502,12 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -518,7 +517,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -544,12 +543,12 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -559,7 +558,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -585,12 +584,12 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -600,7 +599,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -626,12 +625,12 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -641,7 +640,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
@@ -667,12 +666,12 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -682,7 +681,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
@@ -708,12 +707,12 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -723,7 +722,7 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
@@ -749,12 +748,12 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -764,7 +763,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -790,12 +789,12 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -805,7 +804,7 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
@@ -831,12 +830,12 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -846,7 +845,7 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
@@ -872,12 +871,12 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -887,7 +886,7 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
@@ -913,12 +912,12 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -928,7 +927,7 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
@@ -954,12 +953,12 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -969,7 +968,7 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
@@ -995,12 +994,12 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1010,7 +1009,7 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
@@ -1036,12 +1035,12 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1051,7 +1050,7 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
@@ -1077,12 +1076,12 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1092,7 +1091,7 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
@@ -1118,12 +1117,12 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1133,7 +1132,7 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
@@ -1159,12 +1158,12 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1174,7 +1173,7 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
@@ -1200,12 +1199,12 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1215,7 +1214,7 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
@@ -1241,12 +1240,12 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1256,7 +1255,7 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
@@ -1282,12 +1281,12 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1297,7 +1296,7 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
@@ -1323,12 +1322,12 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -1338,7 +1337,7 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
@@ -1364,12 +1363,12 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -1379,7 +1378,7 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
@@ -1405,12 +1404,12 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -1420,7 +1419,7 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
@@ -1446,12 +1445,12 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -1461,7 +1460,7 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
@@ -1487,12 +1486,12 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -1502,7 +1501,7 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
@@ -1528,12 +1527,12 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -1543,7 +1542,7 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
@@ -1569,12 +1568,12 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -1584,7 +1583,7 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
@@ -1610,12 +1609,12 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -1625,7 +1624,7 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
@@ -1651,12 +1650,12 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -1666,7 +1665,7 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
@@ -1692,12 +1691,12 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -1707,7 +1706,7 @@
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
@@ -1733,12 +1732,12 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -1748,7 +1747,7 @@
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
@@ -1774,12 +1773,12 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -1789,7 +1788,7 @@
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
@@ -1815,12 +1814,12 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -1830,7 +1829,7 @@
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
@@ -1856,12 +1855,12 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -1871,7 +1870,7 @@
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
@@ -1897,12 +1896,12 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -1912,7 +1911,7 @@
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
@@ -1938,12 +1937,12 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -1953,7 +1952,7 @@
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
@@ -1979,12 +1978,12 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -1994,7 +1993,7 @@
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
@@ -2020,12 +2019,12 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -2035,7 +2034,7 @@
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
@@ -2061,12 +2060,12 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -2076,7 +2075,7 @@
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
@@ -2102,12 +2101,12 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -2117,7 +2116,7 @@
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
@@ -2143,12 +2142,12 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -2158,7 +2157,7 @@
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
@@ -2184,12 +2183,12 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -2199,7 +2198,7 @@
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
@@ -2225,12 +2224,12 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -2240,7 +2239,7 @@
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
@@ -2266,12 +2265,12 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -2281,7 +2280,7 @@
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
@@ -2307,12 +2306,12 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -2322,7 +2321,7 @@
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
@@ -2348,12 +2347,12 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -2363,7 +2362,7 @@
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
@@ -2389,12 +2388,12 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -2404,7 +2403,7 @@
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
@@ -2430,12 +2429,12 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -2445,7 +2444,7 @@
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
@@ -2471,12 +2470,12 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -2486,7 +2485,7 @@
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H50" t="inlineStr">
@@ -2512,12 +2511,12 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -2527,7 +2526,7 @@
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H51" t="inlineStr">
@@ -2553,12 +2552,12 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -2568,7 +2567,7 @@
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H52" t="inlineStr">
@@ -2594,12 +2593,12 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -2609,7 +2608,7 @@
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H53" t="inlineStr">
@@ -2635,12 +2634,12 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -2650,7 +2649,7 @@
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H54" t="inlineStr">
@@ -2676,12 +2675,12 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -2691,7 +2690,7 @@
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H55" t="inlineStr">
@@ -2717,12 +2716,12 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -2732,7 +2731,7 @@
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H56" t="inlineStr">
@@ -2758,12 +2757,12 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -2773,7 +2772,7 @@
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H57" t="inlineStr">
@@ -2799,12 +2798,12 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -2814,7 +2813,7 @@
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H58" t="inlineStr">
@@ -2840,12 +2839,12 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -2855,7 +2854,7 @@
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H59" t="inlineStr">
@@ -2881,12 +2880,12 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -2896,7 +2895,7 @@
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H60" t="inlineStr">
@@ -2922,12 +2921,12 @@
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -2937,7 +2936,7 @@
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H61" t="inlineStr">
@@ -2963,12 +2962,12 @@
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -2978,7 +2977,7 @@
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H62" t="inlineStr">
@@ -3004,12 +3003,12 @@
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -3019,7 +3018,7 @@
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H63" t="inlineStr">
@@ -3045,12 +3044,12 @@
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -3060,7 +3059,7 @@
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H64" t="inlineStr">
@@ -3086,12 +3085,12 @@
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -3101,7 +3100,7 @@
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H65" t="inlineStr">
@@ -3127,12 +3126,12 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -3142,7 +3141,7 @@
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H66" t="inlineStr">
@@ -3168,12 +3167,12 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -3183,7 +3182,7 @@
       </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H67" t="inlineStr">
@@ -3209,12 +3208,12 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -3224,7 +3223,7 @@
       </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H68" t="inlineStr">
@@ -3250,12 +3249,12 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -3265,7 +3264,7 @@
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H69" t="inlineStr">
@@ -3291,12 +3290,12 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -3306,7 +3305,7 @@
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H70" t="inlineStr">
@@ -3332,12 +3331,12 @@
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -3347,7 +3346,7 @@
       </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H71" t="inlineStr">
@@ -3373,12 +3372,12 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -3388,7 +3387,7 @@
       </c>
       <c r="G72" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H72" t="inlineStr">
@@ -3414,12 +3413,12 @@
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -3429,7 +3428,7 @@
       </c>
       <c r="G73" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H73" t="inlineStr">
@@ -3455,12 +3454,12 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -3470,7 +3469,7 @@
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H74" t="inlineStr">
@@ -3496,12 +3495,12 @@
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -3511,7 +3510,7 @@
       </c>
       <c r="G75" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H75" t="inlineStr">
@@ -3537,12 +3536,12 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -3552,7 +3551,7 @@
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H76" t="inlineStr">
@@ -3578,12 +3577,12 @@
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -3593,7 +3592,7 @@
       </c>
       <c r="G77" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H77" t="inlineStr">
@@ -3619,12 +3618,12 @@
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -3634,7 +3633,7 @@
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H78" t="inlineStr">
@@ -3660,12 +3659,12 @@
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
@@ -3675,7 +3674,7 @@
       </c>
       <c r="G79" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H79" t="inlineStr">
@@ -3701,12 +3700,12 @@
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -3716,7 +3715,7 @@
       </c>
       <c r="G80" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H80" t="inlineStr">
@@ -3742,12 +3741,12 @@
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
@@ -3757,7 +3756,7 @@
       </c>
       <c r="G81" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H81" t="inlineStr">
@@ -3783,12 +3782,12 @@
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
@@ -3798,7 +3797,7 @@
       </c>
       <c r="G82" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H82" t="inlineStr">
@@ -3824,12 +3823,12 @@
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
@@ -3839,7 +3838,7 @@
       </c>
       <c r="G83" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H83" t="inlineStr">
@@ -3865,12 +3864,12 @@
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
@@ -3880,7 +3879,7 @@
       </c>
       <c r="G84" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H84" t="inlineStr">
@@ -3906,12 +3905,12 @@
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
@@ -3921,7 +3920,7 @@
       </c>
       <c r="G85" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H85" t="inlineStr">
@@ -3947,12 +3946,12 @@
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
@@ -3962,7 +3961,7 @@
       </c>
       <c r="G86" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H86" t="inlineStr">
@@ -3988,12 +3987,12 @@
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
@@ -4003,7 +4002,7 @@
       </c>
       <c r="G87" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H87" t="inlineStr">
@@ -4029,12 +4028,12 @@
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
@@ -4044,7 +4043,7 @@
       </c>
       <c r="G88" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H88" t="inlineStr">
@@ -4070,12 +4069,12 @@
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
@@ -4085,7 +4084,7 @@
       </c>
       <c r="G89" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H89" t="inlineStr">
@@ -4111,12 +4110,12 @@
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
@@ -4126,7 +4125,7 @@
       </c>
       <c r="G90" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H90" t="inlineStr">
@@ -4152,12 +4151,12 @@
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
@@ -4167,7 +4166,7 @@
       </c>
       <c r="G91" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H91" t="inlineStr">
@@ -4193,12 +4192,12 @@
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F92" t="inlineStr">
@@ -4208,7 +4207,7 @@
       </c>
       <c r="G92" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H92" t="inlineStr">
@@ -4234,12 +4233,12 @@
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F93" t="inlineStr">
@@ -4249,7 +4248,7 @@
       </c>
       <c r="G93" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H93" t="inlineStr">
@@ -4275,12 +4274,12 @@
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F94" t="inlineStr">
@@ -4290,7 +4289,7 @@
       </c>
       <c r="G94" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H94" t="inlineStr">
@@ -4316,12 +4315,12 @@
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F95" t="inlineStr">
@@ -4331,7 +4330,7 @@
       </c>
       <c r="G95" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H95" t="inlineStr">
@@ -4357,12 +4356,12 @@
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F96" t="inlineStr">
@@ -4372,7 +4371,7 @@
       </c>
       <c r="G96" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H96" t="inlineStr">
@@ -4398,12 +4397,12 @@
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F97" t="inlineStr">
@@ -4413,7 +4412,7 @@
       </c>
       <c r="G97" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H97" t="inlineStr">
@@ -4439,12 +4438,12 @@
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F98" t="inlineStr">
@@ -4454,7 +4453,7 @@
       </c>
       <c r="G98" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H98" t="inlineStr">
@@ -4480,12 +4479,12 @@
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F99" t="inlineStr">
@@ -4495,7 +4494,7 @@
       </c>
       <c r="G99" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H99" t="inlineStr">
@@ -4521,12 +4520,12 @@
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F100" t="inlineStr">
@@ -4536,7 +4535,7 @@
       </c>
       <c r="G100" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H100" t="inlineStr">
@@ -4562,12 +4561,12 @@
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F101" t="inlineStr">
@@ -4577,7 +4576,7 @@
       </c>
       <c r="G101" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H101" t="inlineStr">
@@ -4603,12 +4602,12 @@
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F102" t="inlineStr">
@@ -4618,7 +4617,7 @@
       </c>
       <c r="G102" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H102" t="inlineStr">
@@ -4644,12 +4643,12 @@
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F103" t="inlineStr">
@@ -4659,7 +4658,7 @@
       </c>
       <c r="G103" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H103" t="inlineStr">
@@ -4685,12 +4684,12 @@
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F104" t="inlineStr">
@@ -4700,7 +4699,7 @@
       </c>
       <c r="G104" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H104" t="inlineStr">
@@ -4726,12 +4725,12 @@
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F105" t="inlineStr">
@@ -4741,7 +4740,7 @@
       </c>
       <c r="G105" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H105" t="inlineStr">
@@ -4767,12 +4766,12 @@
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>Loss+DCC</t>
+          <t>GL</t>
         </is>
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>GL</t>
+          <t>Gross</t>
         </is>
       </c>
       <c r="F106" t="inlineStr">
@@ -4782,7 +4781,7 @@
       </c>
       <c r="G106" t="inlineStr">
         <is>
-          <t>Gross</t>
+          <t>Loss+DCC</t>
         </is>
       </c>
       <c r="H106" t="inlineStr">
@@ -5556,7 +5555,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5565,200 +5564,625 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>PAID LOSS</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>period</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>24</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>36</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>48</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
         <is>
           <t>accident_period</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>0</v>
+      </c>
+      <c r="B4" s="3" t="n">
+        <v>40179</v>
+      </c>
+      <c r="C4" t="n">
+        <v>118876786</v>
+      </c>
+      <c r="D4" t="n">
+        <v>239879923.7094306</v>
+      </c>
+      <c r="E4" t="n">
+        <v>337117738.7330799</v>
+      </c>
+      <c r="F4" t="n">
+        <v>425726157.0935614</v>
+      </c>
+      <c r="G4" t="n">
+        <v>492429411.2220569</v>
+      </c>
+      <c r="H4" t="n">
+        <v>515175405.9537438</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>1</v>
+      </c>
+      <c r="B5" s="3" t="n">
+        <v>40544</v>
+      </c>
+      <c r="C5" t="n">
+        <v>125252137</v>
+      </c>
+      <c r="D5" t="n">
+        <v>268528945.4875084</v>
+      </c>
+      <c r="E5" t="n">
+        <v>394613211.0541049</v>
+      </c>
+      <c r="F5" t="n">
+        <v>508312262.8809579</v>
+      </c>
+      <c r="G5" t="n">
+        <v>565734621.7197464</v>
+      </c>
+      <c r="H5" t="n">
+        <v>596756735.3165786</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>2</v>
+      </c>
+      <c r="B6" s="3" t="n">
+        <v>40909</v>
+      </c>
+      <c r="C6" t="n">
+        <v>117085299</v>
+      </c>
+      <c r="D6" t="n">
+        <v>251574715.9342686</v>
+      </c>
+      <c r="E6" t="n">
+        <v>369784388.4749186</v>
+      </c>
+      <c r="F6" t="n">
+        <v>449710389.6885465</v>
+      </c>
+      <c r="G6" t="n">
+        <v>515636700.2471581</v>
+      </c>
+      <c r="H6" t="n">
+        <v>552575474.2471582</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>3</v>
+      </c>
+      <c r="B7" s="3" t="n">
+        <v>41275</v>
+      </c>
+      <c r="C7" t="n">
+        <v>127418922</v>
+      </c>
+      <c r="D7" t="n">
+        <v>275312680.495668</v>
+      </c>
+      <c r="E7" t="n">
+        <v>403367575.8105429</v>
+      </c>
+      <c r="F7" t="n">
+        <v>516540738.618947</v>
+      </c>
+      <c r="G7" t="n">
+        <v>599351854.1531677</v>
+      </c>
+      <c r="H7" t="n">
+        <v>654608915.8197634</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>4</v>
+      </c>
+      <c r="B8" s="3" t="n">
+        <v>41640</v>
+      </c>
+      <c r="C8" t="n">
+        <v>139817284</v>
+      </c>
+      <c r="D8" t="n">
+        <v>321583574.5475294</v>
+      </c>
+      <c r="E8" t="n">
+        <v>497090712.5775042</v>
+      </c>
+      <c r="F8" t="n">
+        <v>668794319.1830169</v>
+      </c>
+      <c r="G8" t="n">
+        <v>798274855.1392238</v>
+      </c>
+      <c r="H8" t="n">
+        <v>850721917.7773768</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>5</v>
+      </c>
+      <c r="B9" s="3" t="n">
+        <v>42005</v>
+      </c>
+      <c r="C9" t="n">
+        <v>86772581.99999997</v>
+      </c>
+      <c r="D9" t="n">
+        <v>208662319.7693367</v>
+      </c>
+      <c r="E9" t="n">
+        <v>331091666.2545342</v>
+      </c>
+      <c r="F9" t="n">
+        <v>445843736.8151995</v>
+      </c>
+      <c r="G9" t="n">
+        <v>517988656.8056653</v>
+      </c>
+      <c r="H9" t="n">
+        <v/>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>REPORTED LOSS</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" t="inlineStr">
         <is>
           <t>period</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C13" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D13" t="inlineStr">
         <is>
           <t>12</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E13" t="inlineStr">
         <is>
           <t>24</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="F13" t="inlineStr">
         <is>
           <t>36</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="G13" t="inlineStr">
         <is>
           <t>48</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="H13" t="inlineStr">
         <is>
           <t>60</t>
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="1" t="n">
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>accident_period</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="n">
+      <c r="B15" s="3" t="n">
         <v>40179</v>
       </c>
-      <c r="C2" t="n">
-        <v>118876786</v>
-      </c>
-      <c r="D2" t="n">
-        <v>239879923.7094306</v>
-      </c>
-      <c r="E2" t="n">
-        <v>337117738.7330799</v>
-      </c>
-      <c r="F2" t="n">
-        <v>425726157.0935614</v>
-      </c>
-      <c r="G2" t="n">
-        <v>492429411.2220569</v>
-      </c>
-      <c r="H2" t="n">
-        <v>515175405.9537438</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="n">
+      <c r="C15" t="n">
+        <v>276824985.6571839</v>
+      </c>
+      <c r="D15" t="n">
+        <v>393168935.4122362</v>
+      </c>
+      <c r="E15" t="n">
+        <v>474086102.3350518</v>
+      </c>
+      <c r="F15" t="n">
+        <v>521134195.1596658</v>
+      </c>
+      <c r="G15" t="n">
+        <v>550194967.0879575</v>
+      </c>
+      <c r="H15" t="n">
+        <v>558419355.8430579</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
         <v>1</v>
       </c>
-      <c r="B3" s="3" t="n">
+      <c r="B16" s="3" t="n">
         <v>40544</v>
       </c>
-      <c r="C3" t="n">
-        <v>125252137</v>
-      </c>
-      <c r="D3" t="n">
-        <v>268528945.4875084</v>
-      </c>
-      <c r="E3" t="n">
-        <v>394613211.0541049</v>
-      </c>
-      <c r="F3" t="n">
-        <v>508312262.8809579</v>
-      </c>
-      <c r="G3" t="n">
-        <v>565734621.7197464</v>
-      </c>
-      <c r="H3" t="n">
-        <v>596756735.3165786</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
+      <c r="C16" t="n">
+        <v>293549997.4855785</v>
+      </c>
+      <c r="D16" t="n">
+        <v>434641131.0381836</v>
+      </c>
+      <c r="E16" t="n">
+        <v>526784103.706218</v>
+      </c>
+      <c r="F16" t="n">
+        <v>588695068.7344806</v>
+      </c>
+      <c r="G16" t="n">
+        <v>609541927.7197464</v>
+      </c>
+      <c r="H16" t="n">
+        <v>620396740.6339705</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
         <v>2</v>
       </c>
-      <c r="B4" s="3" t="n">
+      <c r="B17" s="3" t="n">
         <v>40909</v>
       </c>
-      <c r="C4" t="n">
-        <v>117085299</v>
-      </c>
-      <c r="D4" t="n">
-        <v>251574715.9342686</v>
-      </c>
-      <c r="E4" t="n">
-        <v>369784388.4749186</v>
-      </c>
-      <c r="F4" t="n">
-        <v>449710389.6885465</v>
-      </c>
-      <c r="G4" t="n">
-        <v>515636700.2471581</v>
-      </c>
-      <c r="H4" t="n">
-        <v>552575474.2471582</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
+      <c r="C17" t="n">
+        <v>275396538.7562737</v>
+      </c>
+      <c r="D17" t="n">
+        <v>407926503.1999957</v>
+      </c>
+      <c r="E17" t="n">
+        <v>492153447.6303864</v>
+      </c>
+      <c r="F17" t="n">
+        <v>547005897.1563747</v>
+      </c>
+      <c r="G17" t="n">
+        <v>570758511.2471582</v>
+      </c>
+      <c r="H17" t="n">
+        <v>583056548.0696096</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
         <v>3</v>
       </c>
-      <c r="B5" s="3" t="n">
+      <c r="B18" s="3" t="n">
         <v>41275</v>
       </c>
-      <c r="C5" t="n">
-        <v>127418922</v>
-      </c>
-      <c r="D5" t="n">
-        <v>275312680.495668</v>
-      </c>
-      <c r="E5" t="n">
-        <v>403367575.8105429</v>
-      </c>
-      <c r="F5" t="n">
-        <v>516540738.618947</v>
-      </c>
-      <c r="G5" t="n">
-        <v>599351854.1531677</v>
-      </c>
-      <c r="H5" t="n">
-        <v>654608915.8197634</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
+      <c r="C18" t="n">
+        <v>312776390.3379183</v>
+      </c>
+      <c r="D18" t="n">
+        <v>481070896.2034816</v>
+      </c>
+      <c r="E18" t="n">
+        <v>579633803.5518504</v>
+      </c>
+      <c r="F18" t="n">
+        <v>649025503.2092339</v>
+      </c>
+      <c r="G18" t="n">
+        <v>678454917.6401534</v>
+      </c>
+      <c r="H18" t="n">
+        <v>691234668.5934719</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
         <v>4</v>
       </c>
-      <c r="B6" s="3" t="n">
+      <c r="B19" s="3" t="n">
         <v>41640</v>
       </c>
-      <c r="C6" t="n">
-        <v>139817284</v>
-      </c>
-      <c r="D6" t="n">
-        <v>321583574.5475294</v>
-      </c>
-      <c r="E6" t="n">
-        <v>497090712.5775042</v>
-      </c>
-      <c r="F6" t="n">
-        <v>668794319.1830169</v>
-      </c>
-      <c r="G6" t="n">
-        <v>798274855.1392238</v>
-      </c>
-      <c r="H6" t="n">
-        <v>850721917.7773768</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
+      <c r="C19" t="n">
+        <v>360179077.4012915</v>
+      </c>
+      <c r="D19" t="n">
+        <v>575038016.8109288</v>
+      </c>
+      <c r="E19" t="n">
+        <v>738530341.0753703</v>
+      </c>
+      <c r="F19" t="n">
+        <v>841373432.5439558</v>
+      </c>
+      <c r="G19" t="n">
+        <v>865125943.3189907</v>
+      </c>
+      <c r="H19" t="n">
+        <v>882669899.854508</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
         <v>5</v>
       </c>
-      <c r="B7" s="3" t="n">
+      <c r="B20" s="3" t="n">
         <v>42005</v>
       </c>
-      <c r="C7" t="n">
-        <v>86772581.99999997</v>
-      </c>
-      <c r="D7" t="n">
-        <v>208662319.7693367</v>
-      </c>
-      <c r="E7" t="n">
-        <v>331091666.2545342</v>
-      </c>
-      <c r="F7" t="n">
-        <v>445843736.8151995</v>
-      </c>
-      <c r="G7" t="n">
-        <v>517988656.8056653</v>
-      </c>
-      <c r="H7" t="inlineStr"/>
+      <c r="C20" t="n">
+        <v>236849031.2679058</v>
+      </c>
+      <c r="D20" t="n">
+        <v>388523400.076035</v>
+      </c>
+      <c r="E20" t="n">
+        <v>498943323.307036</v>
+      </c>
+      <c r="F20" t="n">
+        <v>535395398.4391621</v>
+      </c>
+      <c r="G20" t="n">
+        <v>557238227.256027</v>
+      </c>
+      <c r="H20" t="n">
+        <v/>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>EARNED PREMIUM</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>period</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>24</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>36</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>48</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>accident_period</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>0</v>
+      </c>
+      <c r="B26" s="3" t="n">
+        <v>40179</v>
+      </c>
+      <c r="C26" t="n">
+        <v>832029486.03531</v>
+      </c>
+      <c r="D26" t="n">
+        <v>831328315.25607</v>
+      </c>
+      <c r="E26" t="n">
+        <v>830999174.51965</v>
+      </c>
+      <c r="F26" t="n">
+        <v>830997104.85274</v>
+      </c>
+      <c r="G26" t="n">
+        <v>831001104.20218</v>
+      </c>
+      <c r="H26" t="n">
+        <v>830965554.26677</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>1</v>
+      </c>
+      <c r="B27" s="3" t="n">
+        <v>40544</v>
+      </c>
+      <c r="C27" t="n">
+        <v>839767489.28427</v>
+      </c>
+      <c r="D27" t="n">
+        <v>836302249.4663399</v>
+      </c>
+      <c r="E27" t="n">
+        <v>836106060.35255</v>
+      </c>
+      <c r="F27" t="n">
+        <v>836071678.53381</v>
+      </c>
+      <c r="G27" t="n">
+        <v>836518153.6668</v>
+      </c>
+      <c r="H27" t="n">
+        <v>836503495.59545</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>2</v>
+      </c>
+      <c r="B28" s="3" t="n">
+        <v>40909</v>
+      </c>
+      <c r="C28" t="n">
+        <v>831875741.5356899</v>
+      </c>
+      <c r="D28" t="n">
+        <v>828924653.67677</v>
+      </c>
+      <c r="E28" t="n">
+        <v>828592725.33496</v>
+      </c>
+      <c r="F28" t="n">
+        <v>828667580.5871201</v>
+      </c>
+      <c r="G28" t="n">
+        <v>828630254.57971</v>
+      </c>
+      <c r="H28" t="n">
+        <v>828626699.26636</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>3</v>
+      </c>
+      <c r="B29" s="3" t="n">
+        <v>41275</v>
+      </c>
+      <c r="C29" t="n">
+        <v>841492629.97203</v>
+      </c>
+      <c r="D29" t="n">
+        <v>839761586.0268</v>
+      </c>
+      <c r="E29" t="n">
+        <v>839588435.84574</v>
+      </c>
+      <c r="F29" t="n">
+        <v>839534865.78865</v>
+      </c>
+      <c r="G29" t="n">
+        <v>839532506.33181</v>
+      </c>
+      <c r="H29" t="n">
+        <v>839531356.20511</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>4</v>
+      </c>
+      <c r="B30" s="3" t="n">
+        <v>41640</v>
+      </c>
+      <c r="C30" t="n">
+        <v>883006683.4823999</v>
+      </c>
+      <c r="D30" t="n">
+        <v>878318134.07011</v>
+      </c>
+      <c r="E30" t="n">
+        <v>878172934.05829</v>
+      </c>
+      <c r="F30" t="n">
+        <v>878128215.801</v>
+      </c>
+      <c r="G30" t="n">
+        <v>878079725.6378</v>
+      </c>
+      <c r="H30" t="n">
+        <v>878072461.06786</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>5</v>
+      </c>
+      <c r="B31" s="3" t="n">
+        <v>42005</v>
+      </c>
+      <c r="C31" t="n">
+        <v>841268395.33456</v>
+      </c>
+      <c r="D31" t="n">
+        <v>839444887.84718</v>
+      </c>
+      <c r="E31" t="n">
+        <v>839192413.10246</v>
+      </c>
+      <c r="F31" t="n">
+        <v>839106603.53488</v>
+      </c>
+      <c r="G31" t="n">
+        <v>839093187.05159</v>
+      </c>
+      <c r="H31" t="n">
+        <v/>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>